<commit_message>
Add comprehensive setup guide and implementation summary documentation
Co-authored-by: peetee09 <93839860+peetee09@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Ecom_Operations_Tracking_System.xlsx
+++ b/Ecom_Operations_Tracking_System.xlsx
@@ -544,7 +544,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Generated: 2025-10-06 12:10:45</t>
+          <t>Generated: 2025-10-06 12:14:13</t>
         </is>
       </c>
     </row>
@@ -600,7 +600,7 @@
       <c r="D6" s="6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-10-06 12:10</t>
+          <t>2025-10-06 12:14</t>
         </is>
       </c>
     </row>
@@ -622,7 +622,7 @@
       <c r="D7" s="6" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-10-06 12:10</t>
+          <t>2025-10-06 12:14</t>
         </is>
       </c>
     </row>
@@ -644,7 +644,7 @@
       <c r="D8" s="6" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-10-06 12:10</t>
+          <t>2025-10-06 12:14</t>
         </is>
       </c>
     </row>
@@ -666,7 +666,7 @@
       <c r="D9" s="6" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-10-06 12:10</t>
+          <t>2025-10-06 12:14</t>
         </is>
       </c>
     </row>
@@ -688,7 +688,7 @@
       <c r="D10" s="6" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-10-06 12:10</t>
+          <t>2025-10-06 12:14</t>
         </is>
       </c>
     </row>
@@ -710,7 +710,7 @@
       <c r="D11" s="6" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-10-06 12:10</t>
+          <t>2025-10-06 12:14</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-10-06 12:10</t>
+          <t>2025-10-06 12:14</t>
         </is>
       </c>
     </row>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="B3" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 12:10</t>
+          <t>2025-10-06 12:14</t>
         </is>
       </c>
       <c r="C3" s="6" t="inlineStr">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="B4" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 12:10</t>
+          <t>2025-10-06 12:14</t>
         </is>
       </c>
       <c r="C4" s="6" t="inlineStr">
@@ -1275,7 +1275,7 @@
       </c>
       <c r="B5" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 12:10</t>
+          <t>2025-10-06 12:14</t>
         </is>
       </c>
       <c r="C5" s="6" t="inlineStr">
@@ -1671,7 +1671,7 @@
       </c>
       <c r="B3" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 12:10</t>
+          <t>2025-10-06 12:14</t>
         </is>
       </c>
       <c r="C3" s="6" t="inlineStr">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="B4" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 12:10</t>
+          <t>2025-10-06 12:14</t>
         </is>
       </c>
       <c r="C4" s="6" t="inlineStr">
@@ -1775,7 +1775,7 @@
       </c>
       <c r="B5" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 12:10</t>
+          <t>2025-10-06 12:14</t>
         </is>
       </c>
       <c r="C5" s="6" t="inlineStr">
@@ -2452,12 +2452,12 @@
       </c>
       <c r="G3" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 09:10</t>
+          <t>2025-10-06 09:14</t>
         </is>
       </c>
       <c r="H3" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 11:10</t>
+          <t>2025-10-06 11:14</t>
         </is>
       </c>
       <c r="I3" s="6" t="inlineStr">
@@ -2509,12 +2509,12 @@
       </c>
       <c r="G4" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 07:10</t>
+          <t>2025-10-06 07:14</t>
         </is>
       </c>
       <c r="H4" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 12:10</t>
+          <t>2025-10-06 12:14</t>
         </is>
       </c>
       <c r="I4" s="6" t="inlineStr">
@@ -2566,7 +2566,7 @@
       </c>
       <c r="G5" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 10:10</t>
+          <t>2025-10-06 10:14</t>
         </is>
       </c>
       <c r="H5" s="6" t="inlineStr"/>

</xml_diff>

<commit_message>
Create comprehensive Excel-based e-commerce operations tracking system
Co-authored-by: peetee09 <93839860+peetee09@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Ecom_Operations_Tracking_System.xlsx
+++ b/Ecom_Operations_Tracking_System.xlsx
@@ -544,7 +544,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Generated: 2025-10-06 12:14:13</t>
+          <t>Generated: 2025-10-06 12:18:05</t>
         </is>
       </c>
     </row>
@@ -600,7 +600,7 @@
       <c r="D6" s="6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-10-06 12:14</t>
+          <t>2025-10-06 12:18</t>
         </is>
       </c>
     </row>
@@ -622,7 +622,7 @@
       <c r="D7" s="6" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-10-06 12:14</t>
+          <t>2025-10-06 12:18</t>
         </is>
       </c>
     </row>
@@ -644,7 +644,7 @@
       <c r="D8" s="6" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-10-06 12:14</t>
+          <t>2025-10-06 12:18</t>
         </is>
       </c>
     </row>
@@ -666,7 +666,7 @@
       <c r="D9" s="6" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-10-06 12:14</t>
+          <t>2025-10-06 12:18</t>
         </is>
       </c>
     </row>
@@ -688,7 +688,7 @@
       <c r="D10" s="6" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-10-06 12:14</t>
+          <t>2025-10-06 12:18</t>
         </is>
       </c>
     </row>
@@ -710,7 +710,7 @@
       <c r="D11" s="6" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-10-06 12:14</t>
+          <t>2025-10-06 12:18</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-10-06 12:14</t>
+          <t>2025-10-06 12:18</t>
         </is>
       </c>
     </row>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="B3" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 12:14</t>
+          <t>2025-10-06 12:18</t>
         </is>
       </c>
       <c r="C3" s="6" t="inlineStr">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="B4" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 12:14</t>
+          <t>2025-10-06 12:18</t>
         </is>
       </c>
       <c r="C4" s="6" t="inlineStr">
@@ -1275,7 +1275,7 @@
       </c>
       <c r="B5" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 12:14</t>
+          <t>2025-10-06 12:18</t>
         </is>
       </c>
       <c r="C5" s="6" t="inlineStr">
@@ -1671,7 +1671,7 @@
       </c>
       <c r="B3" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 12:14</t>
+          <t>2025-10-06 12:18</t>
         </is>
       </c>
       <c r="C3" s="6" t="inlineStr">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="B4" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 12:14</t>
+          <t>2025-10-06 12:18</t>
         </is>
       </c>
       <c r="C4" s="6" t="inlineStr">
@@ -1775,7 +1775,7 @@
       </c>
       <c r="B5" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 12:14</t>
+          <t>2025-10-06 12:18</t>
         </is>
       </c>
       <c r="C5" s="6" t="inlineStr">
@@ -2452,12 +2452,12 @@
       </c>
       <c r="G3" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 09:14</t>
+          <t>2025-10-06 09:18</t>
         </is>
       </c>
       <c r="H3" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 11:14</t>
+          <t>2025-10-06 11:18</t>
         </is>
       </c>
       <c r="I3" s="6" t="inlineStr">
@@ -2509,12 +2509,12 @@
       </c>
       <c r="G4" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 07:14</t>
+          <t>2025-10-06 07:18</t>
         </is>
       </c>
       <c r="H4" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 12:14</t>
+          <t>2025-10-06 12:18</t>
         </is>
       </c>
       <c r="I4" s="6" t="inlineStr">
@@ -2566,7 +2566,7 @@
       </c>
       <c r="G5" s="6" t="inlineStr">
         <is>
-          <t>2025-10-06 10:14</t>
+          <t>2025-10-06 10:18</t>
         </is>
       </c>
       <c r="H5" s="6" t="inlineStr"/>

</xml_diff>